<commit_message>
Add Cogito experiment logs and update workspace
Added new experiment logs for FillBlank, MultipleChoice, OpenResponse, and TrueFalse tasks under ExperimentLogs. Updated workspace and document layout files to reflect new files and recent activity. Minor changes to AnswerAnalyzer.py and added FleschKincaidTest.py.
</commit_message>
<xml_diff>
--- a/ResultsTable/FindingsTable.xlsx
+++ b/ResultsTable/FindingsTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glipo\Documents\GitHub\NREIP25AP\ResultsTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBB5CBF-AD3F-41FA-9511-98C589EF3068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47042FF2-7D12-4C0D-8BB6-34AAB986FD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3D6D986C-8A2C-4F2D-A60B-C88487A9F56E}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>Model, Attempt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="132">
   <si>
     <t>Correct/Incorrect Length Ratio</t>
   </si>
@@ -47,35 +44,464 @@
     <t>Keyword with highest relative frequency</t>
   </si>
   <si>
-    <t>Highest relative keyword frequency</t>
-  </si>
-  <si>
-    <t>Cogito8B, 0</t>
-  </si>
-  <si>
-    <t>Gemma3NE4B, 0</t>
-  </si>
-  <si>
-    <t>with RAG, 0</t>
-  </si>
-  <si>
-    <t>Granite3.28B, 0</t>
-  </si>
-  <si>
-    <t>Granite3.38B, 0</t>
-  </si>
-  <si>
     <t>Similarity to reference</t>
+  </si>
+  <si>
+    <t>Grading Accuracy (Cogito)</t>
+  </si>
+  <si>
+    <t>with RAG</t>
+  </si>
+  <si>
+    <t>73-90%</t>
+  </si>
+  <si>
+    <t>83-90%</t>
+  </si>
+  <si>
+    <t>73-86%</t>
+  </si>
+  <si>
+    <t>Incorrectly converted fractions to percentages</t>
+  </si>
+  <si>
+    <t>See above</t>
+  </si>
+  <si>
+    <t>Noted and stated (after claiming 19 questions wrong) that questions were vague and poorly worded. Also incorrectly reported a 27/30 out of 30 after claiming five questions wrong.</t>
+  </si>
+  <si>
+    <t>See example 3</t>
+  </si>
+  <si>
+    <t>86%-100%</t>
+  </si>
+  <si>
+    <t>Notes (Gemma)</t>
+  </si>
+  <si>
+    <t>Notes (Cogito)</t>
+  </si>
+  <si>
+    <t>Notes (Granite)</t>
+  </si>
+  <si>
+    <t>Notes (Dolphin)</t>
+  </si>
+  <si>
+    <t>80-97%</t>
+  </si>
+  <si>
+    <t>Has trouble with negation questions (i.e. "which is NOT an example of machine learning?" Also vulnerable to not identifying chosen answers correctly.</t>
+  </si>
+  <si>
+    <t>Gives 30/30 even with a missed question</t>
+  </si>
+  <si>
+    <t>90-100%</t>
+  </si>
+  <si>
+    <t>Really liked deducting 3 questions. After prompting to review, consistently regrades to 100%</t>
+  </si>
+  <si>
+    <t>50-90%</t>
+  </si>
+  <si>
+    <t>Willing to correct back up to 100% after being prompted to review, but is very committed to deducting 3 questions.</t>
+  </si>
+  <si>
+    <t>Decided that questions 6 and 12 were incorrect, despite seeing that the selected answer matched the answer the AI thought was correct. It also at this point attempted suicide.</t>
+  </si>
+  <si>
+    <t>83-86%</t>
+  </si>
+  <si>
+    <t>First instance where the model actually hallucinated somethiing - three questions were totally replaced, marked incorrect, and rewritten. Also wildly miscalculates the final score relative to how many questions were "incorrect." Also has trouble with negations and reading answers, like all other models.</t>
+  </si>
+  <si>
+    <t>80-86%</t>
+  </si>
+  <si>
+    <t>77-100%</t>
+  </si>
+  <si>
+    <t>Repeatedly managed recognize that a question's selected answer was correct before deciding that it was incorrect and supplying an answer it previously believed to be incorrect.</t>
+  </si>
+  <si>
+    <t>56-83%</t>
+  </si>
+  <si>
+    <t>86-93%</t>
+  </si>
+  <si>
+    <t>Some answers chosen were changed by the AI, and then marked incorrect, with the original chosen answer almost always being the correct one. Continued trend of not recognizing selected answers as selected</t>
+  </si>
+  <si>
+    <t>Has an unusual amount of trouble linking the amount of incorrectly answered questions with a fraction. Also totally unable to understand that an particular answer is selected despite explicit instructions.</t>
+  </si>
+  <si>
+    <t>80-96%</t>
+  </si>
+  <si>
+    <t>6-90%</t>
+  </si>
+  <si>
+    <t>Absolutely no idea what happened here. Dolphin simply went off the rails on attempt two and changed its understanding of almost every question. I was not able to replicate this, but I'm not sure it should be excluded as an outlier.</t>
+  </si>
+  <si>
+    <t>13-100%</t>
+  </si>
+  <si>
+    <t>Bizarre redefinition of correct answers continued, but only once and without explanation. In addition, seems to be the weakest model both for identifying correct answers and for converting into a numerical score.</t>
+  </si>
+  <si>
+    <t>First occurance of any model denying that any listed answer is correct.</t>
+  </si>
+  <si>
+    <t>56-93%</t>
+  </si>
+  <si>
+    <t>76-93%</t>
+  </si>
+  <si>
+    <t>Median Score</t>
+  </si>
+  <si>
+    <t>1.5:1</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>1.3:1</t>
+  </si>
+  <si>
+    <t>When marking questions as incorrect, Cogito now actually designates a different answer as being correct. Still occasionally totally misreads the provided exam.</t>
+  </si>
+  <si>
+    <t>36-90%</t>
+  </si>
+  <si>
+    <t>53-90%</t>
+  </si>
+  <si>
+    <t>Occasionally goes totally psychotic and becomes fixated on giving a student a particular score, to the point it reinterprets questions, prompts, and its own thinking to make it fit.</t>
+  </si>
+  <si>
+    <t>47-100%</t>
+  </si>
+  <si>
+    <t>Even when it mismatches answers it thinks is selected and "correct answers", it still gives grades of 100% and believes answers the student (actually) chose are correct.</t>
+  </si>
+  <si>
+    <t>97-100%</t>
+  </si>
+  <si>
+    <t>Flipped a score once from 22/30 to 8/30. Irreplicable.</t>
+  </si>
+  <si>
+    <t>26-100%</t>
+  </si>
+  <si>
+    <t>83-97%</t>
+  </si>
+  <si>
+    <t>Occasionally got confused when trying to point out questions it thought the student got wrong, mixed up numbers</t>
+  </si>
+  <si>
+    <t>Marked some questions consistently wrong, and cited the answer actually chosen as the correct one. Also somehow ended up with 33% score with 10/30 questions missed.</t>
+  </si>
+  <si>
+    <t>66-100%</t>
+  </si>
+  <si>
+    <t>Often flipped around missed and correct answers (before review, would give 6/30 for six questions missed). Also changed what answers it thought the student input, even going so far as to modify the text of the prompt.</t>
+  </si>
+  <si>
+    <t>Again switched which answers were selected.</t>
+  </si>
+  <si>
+    <t>93-100%</t>
+  </si>
+  <si>
+    <t>Matched marked answers recognized them as correct - before immediately changing its mind and saying they are incorrect. Later, it didn't even bother marking answers incorrect before subtracting points.</t>
+  </si>
+  <si>
+    <t>50-100%</t>
+  </si>
+  <si>
+    <t>Changed correctly inputted answers to be false to validate claims that more questions were missed than actually were.</t>
+  </si>
+  <si>
+    <t>See previous column.</t>
+  </si>
+  <si>
+    <t>50-94%</t>
+  </si>
+  <si>
+    <t>Mismatched incorrect answers.</t>
+  </si>
+  <si>
+    <t>56-100%</t>
+  </si>
+  <si>
+    <t>80-100%</t>
+  </si>
+  <si>
+    <t>Hallucinated that three questions were repeats of (totally different) questions.</t>
+  </si>
+  <si>
+    <t>In response to being told it was incorrect, I got accused of lying to the AI.</t>
+  </si>
+  <si>
+    <t>53-94%</t>
+  </si>
+  <si>
+    <t>27-93%</t>
+  </si>
+  <si>
+    <t>Correctly acknowledged selected answers, then unacknowledged them in the same output.</t>
+  </si>
+  <si>
+    <t>Had strong bias because most answers were C.</t>
+  </si>
+  <si>
+    <t>0-100%</t>
+  </si>
+  <si>
+    <t>Misidentified D as A very consistently</t>
+  </si>
+  <si>
+    <t>47-90%</t>
+  </si>
+  <si>
+    <t>Once again had the same idea of what the correct answers were as the generator AI, but changed selected answers to reduce the score. Graded higher when actually forced to compare selected answers and its interpretation of correct answers.</t>
+  </si>
+  <si>
+    <t>36-70%</t>
+  </si>
+  <si>
+    <t>Very consistently had an idea of what the selected answers were. That it was totally incorrect is unrelated but interesting.</t>
+  </si>
+  <si>
+    <t>Unusual response in theform of the AI assigning arbitrary point values (like 23, 25, 5)</t>
+  </si>
+  <si>
+    <t>1.0:1</t>
+  </si>
+  <si>
+    <t>Supervised</t>
+  </si>
+  <si>
+    <t>Networks</t>
+  </si>
+  <si>
+    <t>1.6:1</t>
+  </si>
+  <si>
+    <t>Adaptive</t>
+  </si>
+  <si>
+    <t>1.2:1</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>1.4:1</t>
+  </si>
+  <si>
+    <t>Infinite</t>
+  </si>
+  <si>
+    <t>Patterns</t>
+  </si>
+  <si>
+    <t>Learn</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Short &amp; LSTM</t>
+  </si>
+  <si>
+    <t>Unlabeled, Quality, Quantity</t>
+  </si>
+  <si>
+    <t>Highest keyword frequency</t>
+  </si>
+  <si>
+    <t>Gemma</t>
+  </si>
+  <si>
+    <t>Granite</t>
+  </si>
+  <si>
+    <t>Dolphin</t>
+  </si>
+  <si>
+    <t>Question Type/Attempt</t>
+  </si>
+  <si>
+    <t>Fill-in-the-blank</t>
+  </si>
+  <si>
+    <t>Multiple choice</t>
+  </si>
+  <si>
+    <t>Has a tendency to pull in words from around the input answer when the answer is written in the exam. When it is not, the AI does not recognize that the answer is followed by other words.</t>
+  </si>
+  <si>
+    <t>83-100%</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Completely changes the answer chosen for some questions, often changing them to the point that they are no longereven </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>related</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the original answer or question.</t>
+    </r>
+  </si>
+  <si>
+    <t>56-97%</t>
+  </si>
+  <si>
+    <t>Occasionally does not detect the submitted answer. When it does detect the answer, grading accuracy is higher than average.</t>
+  </si>
+  <si>
+    <t>First instance of any model to correctly identify all answers and grade them correctly every trial.</t>
+  </si>
+  <si>
+    <t>Open Response</t>
+  </si>
+  <si>
+    <t>86-100%</t>
+  </si>
+  <si>
+    <t>More often than not judges the actual student's answers, but occasionally changes what the intended answer is.</t>
+  </si>
+  <si>
+    <t>39-90%</t>
+  </si>
+  <si>
+    <t>The only hallucinations that occurred stemmed from a lack of input, and were able to be quickly corrected.</t>
+  </si>
+  <si>
+    <t>Explicitly ordering the AI to output the question before grading the answer greatly increased performance.</t>
+  </si>
+  <si>
+    <t>True/False</t>
+  </si>
+  <si>
+    <t>Made errors when generating output such as encasing the whole question in parentheses but this did not affect grading. More interestingly, changed format of the questions to be open response while asking generally the same questions.</t>
+  </si>
+  <si>
+    <t>Did not want to or like to ouput the questions before grading them. Then went totally psychotic.</t>
+  </si>
+  <si>
+    <t>70-100%</t>
+  </si>
+  <si>
+    <t>Again started changing answers, even it wrote them out correctly in the question.</t>
+  </si>
+  <si>
+    <t>47-97%</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Retroactively modified the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>correct</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> answer to justify its marking a question wrong.</t>
+    </r>
+  </si>
+  <si>
+    <t>77-93%</t>
+  </si>
+  <si>
+    <t>Went absolutely psychotic counting correct answers.</t>
+  </si>
+  <si>
+    <t>See Cogito. In addition, was extremely lenient and then extremely harsh after being told 30 - 4 does not equal 30.</t>
+  </si>
+  <si>
+    <t>Was extremely unclear in stating whether it actually marked a question correctly or incorrectly. Also routinely gave points when they were not warranted.</t>
+  </si>
+  <si>
+    <t>70-90%</t>
+  </si>
+  <si>
+    <t>Marked multiple questions wrong, then gave a score of 100%</t>
+  </si>
+  <si>
+    <t>90-97%</t>
+  </si>
+  <si>
+    <t>Miscalculated final score, even when provided with all questions it marked incorrectly. Also seems to confuse answers being incorrect for the question having a correct answer of false. Interestingly, gave partial credit to questions without being prompted to.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,8 +527,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,139 +865,782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9681EB4-E878-4F58-BB15-4DE621410D30}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>125</v>
+      </c>
+      <c r="K4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" t="s">
+        <v>127</v>
+      </c>
+      <c r="M4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11">
+        <v>3.18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13">
+        <v>4.18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18">
+        <v>4.5</v>
+      </c>
+      <c r="E18">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" t="s">
+        <v>65</v>
+      </c>
+      <c r="L20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21">
+        <v>3.58</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" t="s">
+        <v>74</v>
+      </c>
+      <c r="J21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" t="s">
+        <v>71</v>
+      </c>
+      <c r="M21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22" t="s">
+        <v>80</v>
+      </c>
+      <c r="M22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="F25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" t="s">
+        <v>107</v>
+      </c>
+      <c r="L25" t="s">
+        <v>109</v>
+      </c>
+      <c r="M25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="F26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" t="s">
+        <v>113</v>
+      </c>
+      <c r="M26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>116</v>
+      </c>
+      <c r="M27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="L29" t="s">
+        <v>121</v>
+      </c>
+      <c r="M29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30">
+        <v>100</v>
+      </c>
+      <c r="G30">
+        <v>100</v>
+      </c>
+      <c r="H30">
+        <v>91</v>
+      </c>
+      <c r="I30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>3</v>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update workspace and add CopilotIndices databases
Added CopilotIndices database files and updated .vs/ProjectSettings.json. Modified workspace paths in DocumentLayout.json to use OneDrive directory. Updated FindingsTable.xlsx and other .vs files to reflect latest changes.
</commit_message>
<xml_diff>
--- a/ResultsTable/FindingsTable.xlsx
+++ b/ResultsTable/FindingsTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glipo\Documents\GitHub\NREIP25AP\ResultsTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/972682759ee0afa5/Documents/GitHub/NREIP25AP/ResultsTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47042FF2-7D12-4C0D-8BB6-34AAB986FD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{47042FF2-7D12-4C0D-8BB6-34AAB986FD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{821D7EC8-A291-460B-B673-E2B6FE58774B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3D6D986C-8A2C-4F2D-A60B-C88487A9F56E}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="138">
   <si>
     <t>Correct/Incorrect Length Ratio</t>
   </si>
@@ -478,6 +476,24 @@
   </si>
   <si>
     <t>Miscalculated final score, even when provided with all questions it marked incorrectly. Also seems to confuse answers being incorrect for the question having a correct answer of false. Interestingly, gave partial credit to questions without being prompted to.</t>
+  </si>
+  <si>
+    <t>56-86%</t>
+  </si>
+  <si>
+    <t>30-70%</t>
+  </si>
+  <si>
+    <t>67-90%</t>
+  </si>
+  <si>
+    <t>77-86%</t>
+  </si>
+  <si>
+    <t>50-80%</t>
+  </si>
+  <si>
+    <t>60-97%</t>
   </si>
 </sst>
 </file>
@@ -868,7 +884,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,6 +983,15 @@
       <c r="F5" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
       <c r="J5" t="s">
         <v>131</v>
       </c>
@@ -975,15 +1000,51 @@
       <c r="A6">
         <v>3</v>
       </c>
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
+      <c r="F7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>